<commit_message>
Tempelate updated for employee master, machine master, machine operator(operator assignment) - updated
</commit_message>
<xml_diff>
--- a/Devoloper_files/sample_template/employee_master.xlsx
+++ b/Devoloper_files/sample_template/employee_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gokulhari\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B45C118-5DC3-451F-B25C-BED66CC6BB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACCD69E-BC2F-4664-A67B-5C6C20D1040D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33810" yWindow="2685" windowWidth="19455" windowHeight="10875" xr2:uid="{6AB8B2EC-B58D-4BFF-BB96-79A584DA8048}"/>
+    <workbookView xWindow="31440" yWindow="2040" windowWidth="22350" windowHeight="13035" xr2:uid="{6AB8B2EC-B58D-4BFF-BB96-79A584DA8048}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,13 +134,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,7 +461,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,81 +478,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>5020</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>9877766547</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I2" s="3"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>5136</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>9877766548</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I3" s="3"/>

</xml_diff>